<commit_message>
Updated operational cybersecurity maturity model
Quick update to the operational model - added some extra flavor text to provide better insights.
</commit_message>
<xml_diff>
--- a/Security Maturity Models - csage.xlsx
+++ b/Security Maturity Models - csage.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csage/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1213ECE8-71E3-6049-B610-8AB0D623B0C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61495DC-6223-6D45-8F1B-5D7DD58B1C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organizational Maturity" sheetId="1" r:id="rId1"/>
     <sheet name="Operational Maturity Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Strategy Sheet" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Example Roadmap" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Likely Change Drivers</t>
   </si>
@@ -83,9 +85,6 @@
     <t>Steady State: Risk-Based</t>
   </si>
   <si>
-    <t>Organizational Security Maturity Model</t>
-  </si>
-  <si>
     <t>Security leadership reports directly to C-Suite and has direct access to the Board of Directors. Security has a budget independent of IT, Ops, Legal.</t>
   </si>
   <si>
@@ -116,24 +115,8 @@
     <t>More Healthy &gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">→→ Changes in regulations, compliance expectations, or industry best practices
-→→ Personnel grows into security and complaince champion, or joins from a more mature organization
-</t>
-  </si>
-  <si>
     <t>← Lack of executive leadership commitment
 ← Lack of attention to changes in regulations, compliance, industry best practices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">→→ Major incident or breach (self or industry peer)
-→→ Shifts in availability or affordability of advanced technology
-→→ Board and leadership prioritize security initiatives and resources
-</t>
-  </si>
-  <si>
-    <t>← Lack of executive leadership commitment
-← Lack of attention to changes in business risk, environment over time
-← Reliance on out-of-date or deprecated technology</t>
   </si>
   <si>
     <r>
@@ -227,9 +210,6 @@
     <t>How Security supports and interacts with the Business</t>
   </si>
   <si>
-    <t>Security Organization</t>
-  </si>
-  <si>
     <t>Operations</t>
   </si>
   <si>
@@ -275,27 +255,6 @@
     <t>Little or no understanding of information security.</t>
   </si>
   <si>
-    <t>BU 2</t>
-  </si>
-  <si>
-    <t>BU 1</t>
-  </si>
-  <si>
-    <t>BU 3</t>
-  </si>
-  <si>
-    <t>BU 4</t>
-  </si>
-  <si>
-    <t>BU 5</t>
-  </si>
-  <si>
-    <t>BU 6</t>
-  </si>
-  <si>
-    <t>BU 7</t>
-  </si>
-  <si>
     <t>Information security efforts lack structure and organization. Even if processes are well defined, they are generally poorly documented. Successful efforts are localized and unlikely to be repeatable or scalable.</t>
   </si>
   <si>
@@ -319,12 +278,92 @@
   <si>
     <t>[Risk-Based, Optimized] 5</t>
   </si>
+  <si>
+    <t>←← Lack of executive leadership commitment
+←← Lack of attention to changes in business risk, environment over time
+←← Reliance on out-of-date or deprecated technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes in regulations, compliance expectations, or industry best practices → 
+Personnel grows into security and complaince champion, or joins from a more mature organization → 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major incident or breach (self or industry peer) →→
+Shifts in availability or affordability of advanced technology →→
+Board and leadership prioritize security initiatives and resources →→
+</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Application Development</t>
+  </si>
+  <si>
+    <t>Service
+Delivery</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Security leadership needs understand how the mission &amp; goals of each BU support the overall organization</t>
+  </si>
+  <si>
+    <t>Compliance shouldn't stand alone; tie it to organizational goals and initiatives.</t>
+  </si>
+  <si>
+    <t>&lt; Example business units; add or remove as needed</t>
+  </si>
+  <si>
+    <t>Determine operational and organizational metrics - the metrics you need to function daily vs. the metrics that demonstrate security's role in achieving organizational goals.</t>
+  </si>
+  <si>
+    <t>Cybersecurity Organization</t>
+  </si>
+  <si>
+    <t>Ensure the tools (technical and non-technical) in use are keeping your cybersecurity team aware and up-to-date with the changing threat landscape for your business, your industry, and informaton security in general.</t>
+  </si>
+  <si>
+    <t>Ensure your cybersecurity team is included in the business' RACI matrices, invited into project discussions early, and that cybersecurity is a key stakeholder in business continuity and disaster recovery plans.</t>
+  </si>
+  <si>
+    <t>How your team identifies and deals with weirdness in your environment, including practice runs, documentation and, when appropriate, engaging law enforcement or the security community at large.</t>
+  </si>
+  <si>
+    <t>Security should understand and have insight into 3rd Party Relationships, whether they're product integrations or vendor platforms.</t>
+  </si>
+  <si>
+    <t>Security should understand the organization's customer base, their needs and how the organization's products/services serve them. Security should be visible/accessible outside of a major incident.</t>
+  </si>
+  <si>
+    <t>How the cybersecurity team addresses security concerns from the general public (social media, good summaritan reporting, news items); participation in bug bounties; visibility within the organization's industry or the security industry.</t>
+  </si>
+  <si>
+    <t>Awareness &amp; Training should be tailored to each specific business unit. Your finance department should be especially aware of phishing and have a direct contact in the security org, for example, but doesn't need to study for the CISSP…</t>
+  </si>
+  <si>
+    <t>Organizational Cybersecurity Maturity Model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -456,7 +495,49 @@
     <font>
       <i/>
       <sz val="10"/>
-      <color theme="1" tint="0.249977111117893"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -742,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -784,27 +865,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -832,18 +892,6 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,39 +901,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,17 +926,147 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="81" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="81" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -924,31 +1078,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="81" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,8 +1309,8 @@
   </sheetPr>
   <dimension ref="B2:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1188,14 +1327,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="18" t="s">
-        <v>20</v>
+      <c r="B2" s="64" t="s">
+        <v>83</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1223,13 +1362,13 @@
     <row r="3" spans="2:30" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="12"/>
       <c r="C3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1257,19 +1396,19 @@
     </row>
     <row r="4" spans="2:30" s="7" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="6"/>
@@ -1300,20 +1439,20 @@
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="25" t="s">
-        <v>30</v>
+      <c r="D5" s="68" t="s">
+        <v>61</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>31</v>
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="2"/>
@@ -1342,15 +1481,15 @@
       <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="26" t="s">
+      <c r="D6" s="68"/>
+      <c r="E6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="29" t="s">
+      <c r="F6" s="68"/>
+      <c r="G6" s="22" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="2"/>
@@ -1381,15 +1520,15 @@
       <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="68"/>
+      <c r="E7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="28" t="s">
+      <c r="F7" s="68"/>
+      <c r="G7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="2"/>
@@ -1420,19 +1559,19 @@
       <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>26</v>
+      <c r="D8" s="69" t="s">
+        <v>24</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>28</v>
+      <c r="F8" s="69" t="s">
+        <v>60</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="2"/>
@@ -1463,16 +1602,16 @@
       <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="70"/>
+      <c r="E9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="30" t="s">
-        <v>21</v>
+      <c r="F9" s="71"/>
+      <c r="G9" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1499,14 +1638,14 @@
       <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="2:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15" t="s">
-        <v>22</v>
+      <c r="B10" s="61" t="s">
+        <v>21</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -32237,357 +32376,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6635C8E3-4B17-CC47-8D4E-419F93CD0ED8}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="42" customWidth="1"/>
-    <col min="2" max="10" width="21.6640625" style="42" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="42"/>
+    <col min="1" max="1" width="28.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="28" customWidth="1"/>
+    <col min="3" max="10" width="10.83203125" style="28" customWidth="1"/>
+    <col min="11" max="11" width="1.83203125" style="50" customWidth="1"/>
+    <col min="12" max="12" width="99.6640625" style="48" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="68" t="s">
+    <row r="1" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="51"/>
+      <c r="L1" s="49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="49"/>
+    </row>
+    <row r="3" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="76"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="49"/>
+    </row>
+    <row r="8" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="78"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="49"/>
+    </row>
+    <row r="12" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="81"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="49"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="49"/>
+    </row>
+    <row r="17" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="41">
+        <v>1</v>
+      </c>
+      <c r="B17" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="49"/>
+    </row>
+    <row r="18" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="49"/>
+    </row>
+    <row r="19" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="49"/>
+    </row>
+    <row r="20" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="49"/>
+    </row>
+    <row r="21" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="68" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
-    </row>
-    <row r="3" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
-    </row>
-    <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
-    </row>
-    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
-    </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="54"/>
-    </row>
-    <row r="9" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
-    </row>
-    <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="54"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
-    </row>
-    <row r="12" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
-    </row>
-    <row r="13" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
-    </row>
-    <row r="14" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="61"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="69">
-        <v>1</v>
-      </c>
-      <c r="B17" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="63"/>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="63"/>
-    </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="63"/>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="63"/>
-    </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="65"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="49"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="L22" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="A16:J16"/>
@@ -32595,11 +32818,31 @@
     <mergeCell ref="B18:J18"/>
     <mergeCell ref="B19:J19"/>
     <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2811DA70-97C6-FB45-97F7-F65C9E97C8B0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998B13C8-7676-1646-90C7-AD0E92DCBFF7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Strategy + Roadmap Examples
Added Example 1st year strategy plan and 4 year roadmap - use these as a starting point for making your strategy & roadmap

Maturity Models: Minor grammar/layout tweaks
</commit_message>
<xml_diff>
--- a/Security Maturity Models - csage.xlsx
+++ b/Security Maturity Models - csage.xlsx
@@ -5,25 +5,133 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csage/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csage/Documents/GitHub/showmethemoney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61495DC-6223-6D45-8F1B-5D7DD58B1C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7411F01-4E24-224F-8A30-241D092195B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="480" windowWidth="29720" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organizational Maturity" sheetId="1" r:id="rId1"/>
     <sheet name="Operational Maturity Model" sheetId="2" r:id="rId2"/>
-    <sheet name="Strategy Sheet" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Example Roadmap" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Carlota Sage</author>
+  </authors>
+  <commentList>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{40E907B9-CFA8-2E47-9EAB-0AEFCAAC6A18}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Carlota Sage:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ensure the tools (technical and non-technical) in use are keeping your cybersecurity team aware and up-to-date with the changing threat landscape for your business, your industry, and informaton security in general.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{97BE6205-67EC-EE4C-9150-30E9179A8F4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Carlota Sage:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>How your team identifies and deals with weirdness in your environment, including practice runs, documentation and, when appropriate, engaging law enforcement or the security community at large.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{B42B63B3-C4E7-B54A-A8D0-C0953B637281}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Carlota Sage:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Your organization shouldn't only hear from Security when something goes wrong; effectively communicating what you do to the different audiences within your organization will increase your overall security posture.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>Likely Change Drivers</t>
   </si>
@@ -203,20 +311,10 @@
     <t>What Business and Security need to know about Regulations</t>
   </si>
   <si>
-    <t>Support &amp;
-Program Mgmt</t>
-  </si>
-  <si>
     <t>How Security supports and interacts with the Business</t>
   </si>
   <si>
-    <t>Operations</t>
-  </si>
-  <si>
     <t>How Security functions</t>
-  </si>
-  <si>
-    <t>Emerging Tech/Threats</t>
   </si>
   <si>
     <t>What Security needs to know about external risk</t>
@@ -241,9 +339,6 @@
   </si>
   <si>
     <t>How Security interacts with external Customers</t>
-  </si>
-  <si>
-    <t>Public Relations</t>
   </si>
   <si>
     <t>How Security presents itself to the public at large</t>
@@ -332,15 +427,6 @@
     <t>Determine operational and organizational metrics - the metrics you need to function daily vs. the metrics that demonstrate security's role in achieving organizational goals.</t>
   </si>
   <si>
-    <t>Cybersecurity Organization</t>
-  </si>
-  <si>
-    <t>Ensure the tools (technical and non-technical) in use are keeping your cybersecurity team aware and up-to-date with the changing threat landscape for your business, your industry, and informaton security in general.</t>
-  </si>
-  <si>
-    <t>Ensure your cybersecurity team is included in the business' RACI matrices, invited into project discussions early, and that cybersecurity is a key stakeholder in business continuity and disaster recovery plans.</t>
-  </si>
-  <si>
     <t>How your team identifies and deals with weirdness in your environment, including practice runs, documentation and, when appropriate, engaging law enforcement or the security community at large.</t>
   </si>
   <si>
@@ -358,12 +444,60 @@
   <si>
     <t>Organizational Cybersecurity Maturity Model</t>
   </si>
+  <si>
+    <t>Communication Strategy</t>
+  </si>
+  <si>
+    <t>Asset Management</t>
+  </si>
+  <si>
+    <t>How Security communicates what's happening</t>
+  </si>
+  <si>
+    <t>Emerging Threats &amp; Vulnerability Mgmt</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Cybersecurity Operations</t>
+  </si>
+  <si>
+    <t>What Security needs to secure</t>
+  </si>
+  <si>
+    <t>How Security monitors assets and environments</t>
+  </si>
+  <si>
+    <t>Communication &amp; Change Management</t>
+  </si>
+  <si>
+    <t>Public Relations &amp; Crisis Communications</t>
+  </si>
+  <si>
+    <t>Program Management</t>
+  </si>
+  <si>
+    <t>Ensure the tools (technical and non-technical) in use are keeping your cybersecurity team aware and up-to-date with the changing threat landscape for your business, your industry, and informaton security in general.</t>
+  </si>
+  <si>
+    <t>While you may not always know what's in your environment, good security hygiene starts with good asset management. Catalogue hardware, software, cloud platforms, devices and data assets on a regular basis, if not continously.</t>
+  </si>
+  <si>
+    <t>Your organization shouldn't only hear from Security when something goes wrong. Ensure your cybersecurity team is included in the business' RACI matrices, invited into project discussions early, and that cybersecurity is a key stakeholder in business continuity and disaster recovery plans.</t>
+  </si>
+  <si>
+    <t>Effectively communicating what you do to the different audiences within your organization will increase your overall security posture.</t>
+  </si>
+  <si>
+    <t>Implement and monitor security controls; establish environmental baseline. Develop detection methods for common/known threats and review detected threats.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -538,6 +672,32 @@
       <i/>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -823,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -898,9 +1058,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -908,23 +1065,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -998,6 +1143,20 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1309,8 +1468,8 @@
   </sheetPr>
   <dimension ref="B2:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1327,14 +1486,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="64" t="s">
-        <v>83</v>
+      <c r="B2" s="65" t="s">
+        <v>76</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1364,9 +1523,9 @@
       <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="14" t="s">
         <v>23</v>
       </c>
@@ -1442,14 +1601,14 @@
       <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="68" t="s">
-        <v>61</v>
+      <c r="D5" s="69" t="s">
+        <v>57</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="68" t="s">
-        <v>62</v>
+      <c r="F5" s="69" t="s">
+        <v>58</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>27</v>
@@ -1484,11 +1643,11 @@
       <c r="C6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="68"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="68"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="22" t="s">
         <v>5</v>
       </c>
@@ -1523,11 +1682,11 @@
       <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="68"/>
+      <c r="D7" s="69"/>
       <c r="E7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="21" t="s">
         <v>9</v>
       </c>
@@ -1562,14 +1721,14 @@
       <c r="C8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="70" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="69" t="s">
-        <v>60</v>
+      <c r="F8" s="70" t="s">
+        <v>56</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>13</v>
@@ -1605,11 +1764,11 @@
       <c r="C9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="70"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="71"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="23" t="s">
         <v>20</v>
       </c>
@@ -1638,14 +1797,14 @@
       <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="2:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="64"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -32375,474 +32534,719 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6635C8E3-4B17-CC47-8D4E-419F93CD0ED8}">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6635C8E3-4B17-CC47-8D4E-419F93CD0ED8}">
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="28" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="28" customWidth="1"/>
-    <col min="3" max="10" width="10.83203125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="1.83203125" style="50" customWidth="1"/>
-    <col min="12" max="12" width="99.6640625" style="48" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="28"/>
+    <col min="1" max="1" width="28.5" style="27" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="60" customWidth="1"/>
+    <col min="3" max="10" width="10.83203125" style="27" customWidth="1"/>
+    <col min="11" max="11" width="1.83203125" style="45" customWidth="1"/>
+    <col min="12" max="12" width="99.6640625" style="43" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="I1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="J1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="46"/>
+      <c r="L1" s="61" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="3" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0</v>
+      </c>
+      <c r="F3" s="28">
+        <v>0</v>
+      </c>
+      <c r="G3" s="28">
+        <v>0</v>
+      </c>
+      <c r="H3" s="28">
+        <v>0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>0</v>
+      </c>
+      <c r="J3" s="28">
+        <v>0</v>
+      </c>
+      <c r="K3" s="48"/>
+      <c r="L3" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0</v>
+      </c>
+      <c r="E4" s="28">
+        <v>0</v>
+      </c>
+      <c r="F4" s="28">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28">
+        <v>0</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0</v>
+      </c>
+      <c r="I4" s="28">
+        <v>0</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0</v>
+      </c>
+      <c r="K4" s="48"/>
+      <c r="L4" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0</v>
+      </c>
+      <c r="E5" s="28">
+        <v>0</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0</v>
+      </c>
+      <c r="G5" s="28">
+        <v>0</v>
+      </c>
+      <c r="H5" s="28">
+        <v>0</v>
+      </c>
+      <c r="I5" s="28">
+        <v>0</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0</v>
+      </c>
+      <c r="K5" s="48"/>
+      <c r="L5" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="28">
+        <v>0</v>
+      </c>
+      <c r="D6" s="28">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28">
+        <v>0</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>0</v>
+      </c>
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>0</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0</v>
+      </c>
+      <c r="K6" s="48"/>
+      <c r="L6" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="44"/>
+    </row>
+    <row r="8" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0</v>
+      </c>
+      <c r="G8" s="28">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
+        <v>0</v>
+      </c>
+      <c r="J8" s="28">
+        <v>0</v>
+      </c>
+      <c r="K8" s="50"/>
+      <c r="L8" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>66</v>
+    </row>
+    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
+        <v>78</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>65</v>
+      <c r="B9" s="58" t="s">
+        <v>83</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>67</v>
+      <c r="C9" s="28">
+        <v>0</v>
       </c>
-      <c r="I1" s="38" t="s">
-        <v>68</v>
+      <c r="D9" s="28">
+        <v>0</v>
       </c>
-      <c r="J1" s="38" t="s">
-        <v>69</v>
+      <c r="E9" s="28">
+        <v>0</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="49" t="s">
+      <c r="F9" s="28">
+        <v>0</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0</v>
+      </c>
+      <c r="K9" s="50"/>
+      <c r="L9" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0</v>
+      </c>
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0</v>
+      </c>
+      <c r="K10" s="50"/>
+      <c r="L10" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0</v>
+      </c>
+      <c r="K11" s="50"/>
+      <c r="L11" s="44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
+        <v>0</v>
+      </c>
+      <c r="J12" s="28">
+        <v>0</v>
+      </c>
+      <c r="K12" s="50"/>
+      <c r="L12" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0</v>
+      </c>
+      <c r="J13" s="28">
+        <v>0</v>
+      </c>
+      <c r="K13" s="50"/>
+      <c r="L13" s="43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="44"/>
+    </row>
+    <row r="15" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0</v>
+      </c>
+      <c r="J15" s="28">
+        <v>0</v>
+      </c>
+      <c r="K15" s="50"/>
+      <c r="L15" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <v>0</v>
+      </c>
+      <c r="G16" s="28">
+        <v>0</v>
+      </c>
+      <c r="H16" s="28">
+        <v>0</v>
+      </c>
+      <c r="I16" s="28">
+        <v>0</v>
+      </c>
+      <c r="J16" s="28">
+        <v>0</v>
+      </c>
+      <c r="K16" s="50"/>
+      <c r="L16" s="44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
-        <v>28</v>
+    <row r="17" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="41" t="s">
+        <v>86</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="49"/>
-    </row>
-    <row r="3" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
-        <v>29</v>
+      <c r="B17" s="42" t="s">
+        <v>45</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>30</v>
+      <c r="C17" s="28">
+        <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="49" t="s">
-        <v>71</v>
+      <c r="D17" s="28">
+        <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
-        <v>31</v>
+      <c r="E17" s="28">
+        <v>0</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>32</v>
+      <c r="F17" s="28">
+        <v>0</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="49" t="s">
-        <v>82</v>
+      <c r="G17" s="28">
+        <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
-        <v>33</v>
+      <c r="H17" s="28">
+        <v>0</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>34</v>
+      <c r="I17" s="28">
+        <v>0</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="49" t="s">
-        <v>72</v>
+      <c r="J17" s="28">
+        <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="49" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="49"/>
-    </row>
-    <row r="8" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="49" t="s">
+      <c r="K17" s="50"/>
+      <c r="L17" s="44" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="49"/>
-    </row>
-    <row r="12" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="82"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="44"/>
+    </row>
+    <row r="20" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36">
+        <v>1</v>
+      </c>
+      <c r="B20" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="49" t="s">
-        <v>80</v>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="44"/>
+    </row>
+    <row r="21" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
+        <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="B21" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>49</v>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="44"/>
+    </row>
+    <row r="22" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
+        <v>51</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="81"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="49"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="84" t="s">
+      <c r="B22" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="49"/>
-    </row>
-    <row r="17" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41">
-        <v>1</v>
-      </c>
-      <c r="B17" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="49"/>
-    </row>
-    <row r="18" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="44"/>
+    </row>
+    <row r="23" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B23" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="49"/>
-    </row>
-    <row r="19" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="44"/>
+    </row>
+    <row r="24" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B24" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="49"/>
-    </row>
-    <row r="20" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="49"/>
-    </row>
-    <row r="21" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="49"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="50"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="L22" s="49"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="44"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="45"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="L25" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="B20:J20"/>
     <mergeCell ref="B21:J21"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2811DA70-97C6-FB45-97F7-F65C9E97C8B0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998B13C8-7676-1646-90C7-AD0E92DCBFF7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>